<commit_message>
Changes regarding retrieving data from excel
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TheGeneral\GitHub\cucumber_Selenium_java\CucumberBaseFramework\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23775" windowHeight="7275"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,208 +26,208 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
   <si>
+    <t>Emailid</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>QuoteState</t>
+  </si>
+  <si>
+    <t>PolicyType</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>PayPlan</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>TimeLifeReferral</t>
+  </si>
+  <si>
+    <t>RoadSideAst</t>
+  </si>
+  <si>
+    <t>HomeOwnerDisc</t>
+  </si>
+  <si>
+    <t>PreviousInsurance</t>
+  </si>
+  <si>
+    <t>DurationOfInsurance</t>
+  </si>
+  <si>
+    <t>PriorBILimits</t>
+  </si>
+  <si>
+    <t>PrimaryInsurance</t>
+  </si>
+  <si>
+    <t>LIBI</t>
+  </si>
+  <si>
+    <t>UMBI</t>
+  </si>
+  <si>
+    <t>UMPD</t>
+  </si>
+  <si>
+    <t>UMPD Ded</t>
+  </si>
+  <si>
+    <t>MedicalPay</t>
+  </si>
+  <si>
+    <t>RentalReim</t>
+  </si>
+  <si>
+    <t>EstimatedCredit</t>
+  </si>
+  <si>
+    <t>CompDed</t>
+  </si>
+  <si>
+    <t>CollDed</t>
+  </si>
+  <si>
+    <t>BusUse</t>
+  </si>
+  <si>
+    <t>DblDed</t>
+  </si>
+  <si>
+    <t>Towing&amp;Labour</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>email1@gmail.com</t>
+  </si>
+  <si>
+    <t>NTVNSV31</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>Bond - No Credit</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>12.5% down, 11 monthly payments</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>Email2@gmail.com</t>
+  </si>
+  <si>
+    <t>NTVNDM31</t>
+  </si>
+  <si>
+    <t>Angular123456</t>
+  </si>
+  <si>
+    <t>Personal Auto - Credit</t>
+  </si>
+  <si>
+    <t>12 months</t>
+  </si>
+  <si>
+    <t>15% down, 11 monthly payments</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>25,000/50,000/15,000</t>
+  </si>
+  <si>
+    <t>25,000/50,000</t>
+  </si>
+  <si>
+    <t>15,000</t>
+  </si>
+  <si>
+    <t>$20 per day / 30 day max</t>
+  </si>
+  <si>
+    <t>Superior</t>
+  </si>
+  <si>
+    <t>$25 per disablement</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Email3@gmail.com</t>
+  </si>
+  <si>
+    <t>6 months</t>
+  </si>
+  <si>
+    <t>Paid-in-full</t>
+  </si>
+  <si>
+    <t>Yes: No lapse (0 days)</t>
+  </si>
+  <si>
+    <t>Less than $50,000/$100,000</t>
+  </si>
+  <si>
+    <t>$30 per day / 30 day max</t>
+  </si>
+  <si>
+    <t>6 months to 1 year</t>
+  </si>
+  <si>
+    <t>5,000</t>
+  </si>
+  <si>
+    <t>$50 per disablement</t>
+  </si>
+  <si>
+    <t>50,000/100,000/50,000</t>
+  </si>
+  <si>
+    <t>50,000/100,000</t>
+  </si>
+  <si>
+    <t>50,000</t>
+  </si>
+  <si>
     <t>Testcaseid</t>
   </si>
   <si>
-    <t>Emailid</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>QuoteState</t>
-  </si>
-  <si>
-    <t>PolicyType</t>
-  </si>
-  <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
-    <t>Term</t>
-  </si>
-  <si>
-    <t>PayPlan</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>TimeLifeReferral</t>
-  </si>
-  <si>
-    <t>RoadSideAst</t>
-  </si>
-  <si>
-    <t>HomeOwnerDisc</t>
-  </si>
-  <si>
-    <t>PreviousInsurance</t>
-  </si>
-  <si>
-    <t>DurationOfInsurance</t>
-  </si>
-  <si>
-    <t>PriorBILimits</t>
-  </si>
-  <si>
-    <t>PrimaryInsurance</t>
-  </si>
-  <si>
-    <t>LIBI</t>
-  </si>
-  <si>
-    <t>UMBI</t>
-  </si>
-  <si>
-    <t>UMPD</t>
-  </si>
-  <si>
-    <t>UMPD Ded</t>
-  </si>
-  <si>
-    <t>MedicalPay</t>
-  </si>
-  <si>
-    <t>RentalReim</t>
-  </si>
-  <si>
-    <t>EstimatedCredit</t>
-  </si>
-  <si>
-    <t>CompDed</t>
-  </si>
-  <si>
-    <t>CollDed</t>
-  </si>
-  <si>
-    <t>BusUse</t>
-  </si>
-  <si>
-    <t>DblDed</t>
-  </si>
-  <si>
-    <t>Towing&amp;Labour</t>
-  </si>
-  <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>email1@gmail.com</t>
-  </si>
-  <si>
-    <t>NTVNSV31</t>
-  </si>
-  <si>
-    <t>welcome19580</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>Bond - No Credit</t>
-  </si>
-  <si>
-    <t>Nil</t>
-  </si>
-  <si>
-    <t>12.5% down, 11 monthly payments</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
-    <t>Email2@gmail.com</t>
-  </si>
-  <si>
-    <t>NTVNDM31</t>
-  </si>
-  <si>
-    <t>Angular123456</t>
-  </si>
-  <si>
-    <t>Personal Auto - Credit</t>
-  </si>
-  <si>
-    <t>12 months</t>
-  </si>
-  <si>
-    <t>15% down, 11 monthly payments</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>25,000/50,000/15,000</t>
-  </si>
-  <si>
-    <t>25,000/50,000</t>
-  </si>
-  <si>
-    <t>15,000</t>
-  </si>
-  <si>
-    <t>$20 per day / 30 day max</t>
-  </si>
-  <si>
-    <t>Superior</t>
-  </si>
-  <si>
-    <t>$25 per disablement</t>
-  </si>
-  <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>Email3@gmail.com</t>
-  </si>
-  <si>
-    <t>NTVNTV30</t>
-  </si>
-  <si>
-    <t>welcome21</t>
-  </si>
-  <si>
-    <t>6 months</t>
-  </si>
-  <si>
-    <t>Paid-in-full</t>
-  </si>
-  <si>
-    <t>Yes: No lapse (0 days)</t>
-  </si>
-  <si>
-    <t>Less than $50,000/$100,000</t>
-  </si>
-  <si>
-    <t>$30 per day / 30 day max</t>
-  </si>
-  <si>
-    <t>6 months to 1 year</t>
-  </si>
-  <si>
-    <t>5,000</t>
-  </si>
-  <si>
-    <t>$50 per disablement</t>
-  </si>
-  <si>
-    <t>50,000/100,000/50,000</t>
-  </si>
-  <si>
-    <t>50,000/100,000</t>
-  </si>
-  <si>
-    <t>50,000</t>
+    <t>welcome2019</t>
+  </si>
+  <si>
+    <t>NTVNSG31</t>
+  </si>
+  <si>
+    <t>sitagabbiti</t>
   </si>
 </sst>
 </file>
@@ -579,272 +583,273 @@
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
     <col min="14" max="14" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2">
+        <v>37209</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="2">
-        <v>37214</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="G3" s="2">
         <v>37214</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="M3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="S3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="2" t="s">
+      <c r="T3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="U3" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="V3" s="2">
         <v>500</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Y3" s="2">
         <v>250</v>
@@ -853,87 +858,87 @@
         <v>250</v>
       </c>
       <c r="AA3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2">
         <v>37214</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="X4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Y4" s="2">
         <v>1500</v>
@@ -942,13 +947,13 @@
         <v>1500</v>
       </c>
       <c r="AA4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added QuoteSearch step and pages.Also made minor changes
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
data writing to excel code is added
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TheGeneral\GitHub\cucumber_Selenium_java\CucumberBaseFramework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23775" windowHeight="7275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23775" windowHeight="7275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
   <si>
     <t>Emailid</t>
   </si>
@@ -240,13 +241,41 @@
   </si>
   <si>
     <t>Restricted</t>
+  </si>
+  <si>
+    <t>TN2485269</t>
+  </si>
+  <si>
+    <t>11538380</t>
+  </si>
+  <si>
+    <t>TB2485272</t>
+  </si>
+  <si>
+    <t>11538402</t>
+  </si>
+  <si>
+    <t>Policy Number</t>
+  </si>
+  <si>
+    <t>Quote Number</t>
+  </si>
+  <si>
+    <t>Type Policy</t>
+  </si>
+  <si>
+    <t>TB2485273</t>
+  </si>
+  <si>
+    <t>11538440</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,23 +623,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="14" max="14" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="19.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -978,4 +1005,72 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="15.42578125" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
business questions code is updated
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23775" windowHeight="7275" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="84">
   <si>
     <t>Emailid</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t xml:space="preserve">Policy Type </t>
+  </si>
+  <si>
+    <t>TC004</t>
   </si>
 </sst>
 </file>
@@ -626,9 +629,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1001,14 +1006,104 @@
         <v>60</v>
       </c>
     </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1016,7 +1111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
2Drivers supporting code is added
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TheGeneral\GitHub\cucumber_Selenium_java\CucumberBaseFramework\src\test\resources\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27690" windowHeight="10695"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="86">
   <si>
     <t>Emailid</t>
   </si>
@@ -277,6 +273,12 @@
   </si>
   <si>
     <t>TC004</t>
+  </si>
+  <si>
+    <t>AdditionalDriver</t>
+  </si>
+  <si>
+    <t>TC005</t>
   </si>
 </sst>
 </file>
@@ -629,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,10 +649,11 @@
     <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -738,8 +741,11 @@
       <c r="AC1" t="s">
         <v>27</v>
       </c>
+      <c r="AD1" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -827,8 +833,11 @@
       <c r="AC2" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="AD2" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" customFormat="1" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -916,8 +925,11 @@
       <c r="AC3" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="AD3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1005,8 +1017,11 @@
       <c r="AC4" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="AD4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -1093,6 +1108,101 @@
       </c>
       <c r="AC5" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" customFormat="1" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1101,9 +1211,10 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
small changes for bus_use
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TheGeneral\GitHub\cucumber_Selenium_java\CucumberBaseFramework\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27690" windowHeight="10695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="90">
   <si>
     <t>Emailid</t>
   </si>
@@ -279,13 +283,25 @@
   </si>
   <si>
     <t>TC005</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>1FTSW21P97EB36008</t>
+  </si>
+  <si>
+    <t>1D7HU182X7J636261</t>
+  </si>
+  <si>
+    <t>1D7HA18P97J504239</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +329,12 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF032F62"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -335,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -350,6 +372,10 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -631,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,11 +675,13 @@
     <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="24.28515625" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" customWidth="1"/>
+    <col min="23" max="23" width="25" customWidth="1"/>
+    <col min="30" max="30" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -721,72 +749,75 @@
         <v>20</v>
       </c>
       <c r="W1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>68</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>33</v>
@@ -795,60 +826,63 @@
         <v>33</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>33</v>
+        <v>33</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>35</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AD2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:30" customFormat="1" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>31</v>
@@ -860,76 +894,79 @@
         <v>68</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>47</v>
+        <v>61</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>33</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="X3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Y3" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="Z3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB3" t="s">
         <v>35</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -996,43 +1033,46 @@
       <c r="V4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="W4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="Y4" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="Y4" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="Z4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AA4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>35</v>
+      <c r="AA4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="AC4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>31</v>
@@ -1044,117 +1084,120 @@
         <v>68</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>71</v>
+        <v>41</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>63</v>
+        <v>45</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="U5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="X5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Y5" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="Z5" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE5" t="s">
         <v>44</v>
       </c>
-      <c r="AB5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="6" spans="1:30" customFormat="1" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
         <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>68</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>33</v>
@@ -1163,55 +1206,58 @@
         <v>33</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="U6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
thread.sleep is added and feature files are updated
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="102">
   <si>
     <t>Emailid</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Testcaseid</t>
   </si>
   <si>
-    <t>welcome2019</t>
-  </si>
-  <si>
     <t>NTVNSG31</t>
   </si>
   <si>
@@ -295,6 +292,45 @@
   </si>
   <si>
     <t>1D7HA18P97J504239</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>DL</t>
+  </si>
+  <si>
+    <t>666195140</t>
+  </si>
+  <si>
+    <t>487956891</t>
+  </si>
+  <si>
+    <t>666195141</t>
+  </si>
+  <si>
+    <t>666195142</t>
+  </si>
+  <si>
+    <t>666195143</t>
+  </si>
+  <si>
+    <t>487956892</t>
+  </si>
+  <si>
+    <t>487956893</t>
+  </si>
+  <si>
+    <t>487956894</t>
+  </si>
+  <si>
+    <t>htcglobal2019</t>
+  </si>
+  <si>
+    <t>666195144</t>
+  </si>
+  <si>
+    <t>487956895</t>
   </si>
 </sst>
 </file>
@@ -657,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,13 +711,13 @@
     <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.85546875" customWidth="1"/>
-    <col min="23" max="23" width="25" customWidth="1"/>
-    <col min="30" max="30" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.28515625" customWidth="1"/>
+    <col min="22" max="24" width="16.85546875" customWidth="1"/>
+    <col min="25" max="25" width="25" customWidth="1"/>
+    <col min="32" max="32" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -749,34 +785,40 @@
         <v>20</v>
       </c>
       <c r="W1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="X1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" t="s">
-        <v>84</v>
+      <c r="AG1" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -796,7 +838,7 @@
         <v>40</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>41</v>
@@ -841,37 +883,43 @@
         <v>33</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="X2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AB2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -879,10 +927,10 @@
         <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>31</v>
@@ -891,7 +939,7 @@
         <v>40</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>53</v>
@@ -900,7 +948,7 @@
         <v>54</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
@@ -938,35 +986,41 @@
       <c r="V3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="W3" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="X3" s="2" t="s">
+      <c r="W3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AB3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -974,10 +1028,10 @@
         <v>52</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>31</v>
@@ -986,7 +1040,7 @@
         <v>40</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>53</v>
@@ -995,7 +1049,7 @@
         <v>54</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>35</v>
@@ -1033,37 +1087,43 @@
       <c r="V4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="W4" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="X4" s="2" t="s">
+      <c r="W4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="AA4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Z4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA4" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="AB4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AC4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>37</v>
@@ -1081,7 +1141,7 @@
         <v>40</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>41</v>
@@ -1126,39 +1186,45 @@
         <v>33</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W5" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="X5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Y5" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Z5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AB5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
@@ -1167,7 +1233,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -1176,7 +1242,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>33</v>
@@ -1223,11 +1289,11 @@
       <c r="V6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>33</v>
+      <c r="W6" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="Y6" s="2" t="s">
         <v>33</v>
@@ -1248,6 +1314,12 @@
         <v>33</v>
       </c>
       <c r="AE6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG6" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1283,13 +1355,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1300,26 +1372,26 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
         <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
         <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
         <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -1327,16 +1399,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
update username and password
update username and password
</commit_message>
<xml_diff>
--- a/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
+++ b/CucumberBaseFramework/src/test/resources/TestData/Datadriven1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="103">
   <si>
     <t>Emailid</t>
   </si>
@@ -217,12 +217,6 @@
   </si>
   <si>
     <t>Testcaseid</t>
-  </si>
-  <si>
-    <t>NTVNSG31</t>
-  </si>
-  <si>
-    <t>sitagabbiti</t>
   </si>
   <si>
     <t>37209</t>
@@ -704,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,13 +788,13 @@
         <v>20</v>
       </c>
       <c r="W1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="X1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Y1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Z1" t="s">
         <v>21</v>
@@ -824,7 +818,7 @@
         <v>27</v>
       </c>
       <c r="AG1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="48.75" x14ac:dyDescent="0.25">
@@ -838,7 +832,7 @@
         <v>38</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>31</v>
@@ -847,7 +841,7 @@
         <v>39</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>40</v>
@@ -892,16 +886,16 @@
         <v>33</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>47</v>
@@ -910,10 +904,10 @@
         <v>48</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AD2" t="s">
         <v>35</v>
@@ -936,10 +930,10 @@
         <v>51</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>31</v>
@@ -948,7 +942,7 @@
         <v>39</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>52</v>
@@ -957,7 +951,7 @@
         <v>53</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
@@ -996,13 +990,13 @@
         <v>58</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="X3" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Y3" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>56</v>
@@ -1011,10 +1005,10 @@
         <v>48</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AC3" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AD3" t="s">
         <v>35</v>
@@ -1037,10 +1031,10 @@
         <v>51</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>31</v>
@@ -1049,7 +1043,7 @@
         <v>39</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>52</v>
@@ -1058,7 +1052,7 @@
         <v>53</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>35</v>
@@ -1097,13 +1091,13 @@
         <v>58</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Y4" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z4" s="2" t="s">
         <v>56</v>
@@ -1112,10 +1106,10 @@
         <v>48</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AD4" s="7" t="s">
         <v>43</v>
@@ -1132,7 +1126,7 @@
     </row>
     <row r="5" spans="1:33" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>37</v>
@@ -1141,7 +1135,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>31</v>
@@ -1150,7 +1144,7 @@
         <v>39</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>40</v>
@@ -1195,16 +1189,16 @@
         <v>33</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Y5" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>47</v>
@@ -1213,10 +1207,10 @@
         <v>48</v>
       </c>
       <c r="AB5" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AC5" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AD5" t="s">
         <v>35</v>
@@ -1233,7 +1227,7 @@
     </row>
     <row r="6" spans="1:33" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
@@ -1242,7 +1236,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -1251,7 +1245,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>33</v>
@@ -1299,10 +1293,10 @@
         <v>33</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Y6" s="2" t="s">
         <v>33</v>
@@ -1334,7 +1328,7 @@
     </row>
     <row r="7" spans="1:33" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>29</v>
@@ -1343,7 +1337,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
         <v>31</v>
@@ -1352,7 +1346,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>33</v>
@@ -1400,10 +1394,10 @@
         <v>33</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Y7" s="2" t="s">
         <v>33</v>
@@ -1435,7 +1429,7 @@
     </row>
     <row r="8" spans="1:33" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>29</v>
@@ -1444,7 +1438,7 @@
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
         <v>31</v>
@@ -1453,7 +1447,7 @@
         <v>32</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>33</v>
@@ -1501,10 +1495,10 @@
         <v>33</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="X8" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Y8" s="2" t="s">
         <v>33</v>
@@ -1536,7 +1530,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -1545,7 +1539,7 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
         <v>31</v>
@@ -1669,13 +1663,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1686,26 +1680,26 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -1713,16 +1707,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>50</v>

</xml_diff>